<commit_message>
Added ground station code
</commit_message>
<xml_diff>
--- a/documentation/bom.xlsx
+++ b/documentation/bom.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtc0030/Documents/Projects/HAB/ros-hab-dcs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtc0030/Documents/Projects/HAB/ros-hab-dcs/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA470B1-05F0-0C4A-8DAA-34A038C47F34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3EDA098-F143-2A44-814A-091FABAAA075}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19480" xr2:uid="{9E5CD0A4-BAAD-3342-BAB6-1E57A22FEC73}"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
-    <sheet name="Shipping Numbers" sheetId="2" r:id="rId2"/>
+    <sheet name="Unused Materials" sheetId="4" r:id="rId2"/>
+    <sheet name="Shipping Numbers" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="183">
   <si>
     <t>Component</t>
   </si>
@@ -43,9 +44,6 @@
     <t>URL</t>
   </si>
   <si>
-    <t>IMU</t>
-  </si>
-  <si>
     <t>Barometer</t>
   </si>
   <si>
@@ -497,6 +495,87 @@
   </si>
   <si>
     <t>"9200190106460345687311"</t>
+  </si>
+  <si>
+    <t>Raspberry Pi Zero</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/3400</t>
+  </si>
+  <si>
+    <t>Digikey (IMU &amp; Arduino)</t>
+  </si>
+  <si>
+    <t>"9200190106460345897567"</t>
+  </si>
+  <si>
+    <t>Amazon (Reg &amp; GPS Antenna)</t>
+  </si>
+  <si>
+    <t>"9374889728009055422404"</t>
+  </si>
+  <si>
+    <t>Short Range Transciever</t>
+  </si>
+  <si>
+    <t>https://amz.run/43zo</t>
+  </si>
+  <si>
+    <t>nRF24L01</t>
+  </si>
+  <si>
+    <t>Protoboard Parts</t>
+  </si>
+  <si>
+    <t>https://amz.run/43zq</t>
+  </si>
+  <si>
+    <t>Universal PCB Board Kit</t>
+  </si>
+  <si>
+    <t>Waterproof GPS Active Antenna 28dB Gain</t>
+  </si>
+  <si>
+    <t>GPS Antenna</t>
+  </si>
+  <si>
+    <t>https://amz.run/43zu</t>
+  </si>
+  <si>
+    <t>Regulator</t>
+  </si>
+  <si>
+    <t>https://amz.run/43zy</t>
+  </si>
+  <si>
+    <t>Pololu 5V, 5A Step-Down Voltage Regulator D24V50F5</t>
+  </si>
+  <si>
+    <t>IMU 1</t>
+  </si>
+  <si>
+    <t>IMU 2</t>
+  </si>
+  <si>
+    <t>9DOF IMU BREAKOUT - ICM-20948</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/sparkfun-electronics/SEN-15335/10279707</t>
+  </si>
+  <si>
+    <t>Arduino</t>
+  </si>
+  <si>
+    <t>Arduino Nano</t>
+  </si>
+  <si>
+    <t>US/China</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/dfrobot/DFR0010/6588448?s=N4IgjCBcoJwBwBYqgMZQGYEMA2BnApgDQgD2UA2iAMxgBsADAEz0gC6xADgC5QgDKXAE4BLAHYBzEAF9iAWiTQQaSFjxFSFcGADsYOG049IIaTJCNNmQQBMArmJIACUZlFlWUoA</t>
+  </si>
+  <si>
+    <t>Shipping</t>
   </si>
 </sst>
 </file>
@@ -671,7 +750,157 @@
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1012,10 +1241,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98B9A57A-E0D4-A741-AAF6-B0573DD3DFDF}">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1036,7 +1265,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="26" t="s">
         <v>1</v>
@@ -1045,19 +1274,19 @@
         <v>2</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F1" s="26" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H1" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I1" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J1" s="26" t="s">
         <v>4</v>
@@ -1065,1157 +1294,1309 @@
     </row>
     <row r="2" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F2" s="29">
         <v>35</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H2" s="29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I2" s="30">
         <v>75</v>
       </c>
       <c r="J2" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F3" s="13">
         <v>0</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I3" s="14">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="F4" s="16">
+      <c r="A4" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="32">
+        <v>7.98</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="17">
+        <v>15</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="16">
         <f>18.49*2</f>
         <v>36.979999999999997</v>
       </c>
-      <c r="G4" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="17">
+      <c r="G5" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="17">
         <v>0.25</v>
       </c>
-      <c r="J4" s="18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="F5" s="16">
-        <v>29.99</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="17">
-        <v>30</v>
-      </c>
-      <c r="J5" s="15" t="s">
-        <v>69</v>
+      <c r="J5" s="18" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F6" s="16">
-        <v>29</v>
+        <v>29.99</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I6" s="17">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>73</v>
+        <v>12</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>74</v>
+        <v>17</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>106</v>
+        <v>10</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>94</v>
       </c>
       <c r="F7" s="16">
-        <v>4.07</v>
+        <v>29</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I7" s="17">
-        <v>10</v>
-      </c>
-      <c r="J7" s="18" t="s">
-        <v>88</v>
+        <v>5</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>71</v>
+        <v>178</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>72</v>
+        <v>179</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>94</v>
+        <v>180</v>
       </c>
       <c r="F8" s="16">
-        <v>5.95</v>
+        <v>19.5</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>109</v>
+        <v>182</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I8" s="17">
-        <v>10</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>98</v>
+        <v>5</v>
+      </c>
+      <c r="J8" s="18" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>147</v>
+        <v>71</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="F9" s="16">
-        <v>35</v>
+        <v>5.95</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I9" s="17">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>148</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>149</v>
+        <v>7</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F10" s="16">
-        <v>7.95</v>
+        <v>35</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I10" s="17">
-        <v>0</v>
-      </c>
-      <c r="J10" s="18" t="s">
-        <v>151</v>
+        <v>20</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>5</v>
+        <v>148</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>7</v>
+        <v>149</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>94</v>
+        <v>126</v>
       </c>
       <c r="F11" s="16">
-        <v>19.95</v>
+        <v>7.95</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I11" s="17">
-        <v>5</v>
-      </c>
-      <c r="J11" s="15" t="s">
-        <v>99</v>
+        <v>0</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>6</v>
+        <v>171</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>110</v>
+        <v>173</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>94</v>
       </c>
       <c r="F12" s="16">
-        <v>0</v>
+        <v>16.36</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I12" s="17">
         <v>5</v>
       </c>
-      <c r="J12" s="15" t="s">
-        <v>102</v>
+      <c r="J12" s="18" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="31" t="s">
-        <v>12</v>
+      <c r="A13" s="15" t="s">
+        <v>174</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="E13" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="F13" s="32">
-        <v>39.99</v>
+        <v>21</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13" s="16">
+        <v>19.95</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I13" s="17">
-        <v>10</v>
-      </c>
-      <c r="J13" s="18" t="s">
-        <v>101</v>
+        <v>5</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>14</v>
+        <v>175</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>15</v>
+        <v>176</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="F14" s="16">
-        <v>60.49</v>
+        <v>16.95</v>
       </c>
       <c r="G14" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="17">
+        <v>5</v>
+      </c>
+      <c r="J14" s="18" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="H14" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" s="17">
+      <c r="D15" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15" s="16">
+        <v>0</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H15" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="15" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="D15" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="E15" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="F15" s="32">
-        <v>33.19</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="H15" s="16" t="s">
-        <v>21</v>
-      </c>
       <c r="I15" s="17">
-        <v>10</v>
-      </c>
-      <c r="J15" s="18" t="s">
-        <v>104</v>
+        <v>5</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>35</v>
+        <v>162</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>37</v>
+        <v>164</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>94</v>
       </c>
       <c r="F16" s="16">
-        <v>129.99</v>
+        <v>0</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I16" s="17">
-        <v>114</v>
-      </c>
-      <c r="J16" s="18" t="s">
-        <v>36</v>
+        <v>5</v>
+      </c>
+      <c r="J16" s="15" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>38</v>
+        <v>165</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>41</v>
+        <v>167</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="15" t="s">
         <v>94</v>
       </c>
       <c r="F17" s="16">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H17" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I17" s="17">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>39</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="15" t="s">
-        <v>80</v>
+      <c r="A18" s="31" t="s">
+        <v>11</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="F18" s="16">
-        <v>7.99</v>
+        <v>21</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="F18" s="32">
+        <v>39.99</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I18" s="17">
-        <v>5</v>
-      </c>
-      <c r="J18" s="15" t="s">
-        <v>81</v>
+        <v>10</v>
+      </c>
+      <c r="J18" s="18" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="15" t="s">
-        <v>85</v>
+      <c r="A19" s="31" t="s">
+        <v>169</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>11</v>
+        <v>21</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>10</v>
       </c>
       <c r="E19" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="F19" s="16">
-        <v>11.99</v>
+        <v>94</v>
+      </c>
+      <c r="F19" s="32">
+        <v>14.99</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I19" s="17">
-        <v>10</v>
-      </c>
-      <c r="J19" s="15" t="s">
-        <v>86</v>
+        <v>20</v>
+      </c>
+      <c r="J19" s="18" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>11</v>
+        <v>127</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
       <c r="F20" s="16">
-        <v>5.98</v>
+        <v>60.49</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I20" s="17">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>53</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="31" t="s">
-        <v>94</v>
+        <v>10</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>93</v>
       </c>
       <c r="F21" s="16">
-        <v>15.98</v>
+        <v>129.99</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I21" s="17">
-        <f>23*4</f>
-        <v>92</v>
-      </c>
-      <c r="J21" s="15" t="s">
-        <v>52</v>
+        <v>114</v>
+      </c>
+      <c r="J21" s="18" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="E22" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="F22" s="16">
+        <v>50</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I22" s="17">
+        <v>0</v>
+      </c>
+      <c r="J22" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="F22" s="16">
-        <v>12.96</v>
-      </c>
-      <c r="G22" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="H22" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="I22" s="17">
-        <v>400</v>
-      </c>
-      <c r="J22" s="34" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="D23" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="F23" s="32">
-        <v>13.99</v>
+      <c r="F23" s="16">
+        <v>7.99</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I23" s="17">
-        <v>20</v>
-      </c>
-      <c r="J23" s="18" t="s">
-        <v>64</v>
+        <v>5</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="31" t="s">
         <v>94</v>
       </c>
       <c r="F24" s="16">
+        <v>11.99</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I24" s="17">
+        <v>10</v>
+      </c>
+      <c r="J24" s="15" t="s">
         <v>85</v>
-      </c>
-      <c r="G24" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="H24" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="I24" s="17">
-        <v>0</v>
-      </c>
-      <c r="J24" s="15" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="B25" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" s="16">
+        <v>5.98</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H25" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="F25" s="16">
-        <v>15.99</v>
-      </c>
-      <c r="G25" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="H25" s="16" t="s">
-        <v>25</v>
-      </c>
       <c r="I25" s="17">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J25" s="15" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B26" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="F26" s="16">
+        <v>15.98</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H26" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="15" t="s">
+      <c r="I26" s="17">
+        <f>23*6</f>
+        <v>138</v>
+      </c>
+      <c r="J26" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F27" s="16">
+        <v>12.96</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27" s="17">
+        <v>400</v>
+      </c>
+      <c r="J27" s="34" t="s">
         <v>95</v>
-      </c>
-      <c r="F26" s="16">
-        <v>9.89</v>
-      </c>
-      <c r="G26" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="H26" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="I26" s="17">
-        <v>10</v>
-      </c>
-      <c r="J26" s="15" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="F27" s="32">
-        <v>9.19</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="H27" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="I27" s="17">
-        <v>5</v>
-      </c>
-      <c r="J27" s="18" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="31" t="s">
-        <v>130</v>
+        <v>64</v>
       </c>
       <c r="B28" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" s="32">
+        <v>13.99</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I28" s="17">
+        <v>20</v>
+      </c>
+      <c r="J28" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F29" s="16">
+        <v>85</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I29" s="17">
+        <v>0</v>
+      </c>
+      <c r="J29" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="D28" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="F28" s="32">
-        <v>9.99</v>
-      </c>
-      <c r="G28" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="H28" s="16" t="s">
+      <c r="B30" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="I28" s="17">
-        <v>5</v>
-      </c>
-      <c r="J28" s="18" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="D29" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="F29" s="32">
-        <v>7.98</v>
-      </c>
-      <c r="G29" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="H29" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="I29" s="17">
-        <v>5</v>
-      </c>
-      <c r="J29" s="18" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="31" t="s">
-        <v>137</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C30" s="31" t="s">
-        <v>138</v>
-      </c>
-      <c r="D30" s="31" t="s">
-        <v>139</v>
+      <c r="D30" s="15" t="s">
+        <v>10</v>
       </c>
       <c r="E30" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="F30" s="32">
-        <v>12.56</v>
+      <c r="F30" s="16">
+        <v>15.99</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I30" s="17">
-        <v>15</v>
-      </c>
-      <c r="J30" s="18" t="s">
-        <v>140</v>
+        <v>10</v>
+      </c>
+      <c r="J30" s="15" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="31" t="s">
-        <v>141</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" s="31" t="s">
-        <v>146</v>
-      </c>
-      <c r="D31" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="E31" s="31" t="s">
+      <c r="A31" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="F31" s="32">
-        <v>3.77</v>
+      <c r="F31" s="16">
+        <v>9.89</v>
       </c>
       <c r="G31" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I31" s="17">
-        <v>5</v>
-      </c>
-      <c r="J31" s="18" t="s">
-        <v>142</v>
+        <v>10</v>
+      </c>
+      <c r="J31" s="15" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="31" t="s">
-        <v>144</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>22</v>
+        <v>65</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>145</v>
+        <v>67</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>97</v>
+        <v>10</v>
       </c>
       <c r="E32" s="31" t="s">
         <v>94</v>
       </c>
       <c r="F32" s="32">
-        <v>1.29</v>
+        <v>9.19</v>
       </c>
       <c r="G32" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H32" s="16" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I32" s="17">
         <v>5</v>
       </c>
       <c r="J32" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="D33" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="F33" s="32">
+        <v>9.99</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H33" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I33" s="17">
+        <v>5</v>
+      </c>
+      <c r="J33" s="18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="D34" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="E34" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="F34" s="32">
+        <v>12.56</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H34" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I34" s="17">
+        <v>15</v>
+      </c>
+      <c r="J34" s="18" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="D35" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="E35" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="F35" s="32">
+        <v>3.77</v>
+      </c>
+      <c r="G35" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H35" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I35" s="17">
+        <v>5</v>
+      </c>
+      <c r="J35" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="31" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C33" s="15" t="s">
+      <c r="B36" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="D36" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="E36" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="F36" s="32">
+        <v>1.29</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H36" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I36" s="17">
+        <v>5</v>
+      </c>
+      <c r="J36" s="18" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F37" s="16">
+        <v>60</v>
+      </c>
+      <c r="G37" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H37" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I37" s="17">
+        <v>0</v>
+      </c>
+      <c r="J37" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" s="22" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="F38" s="23">
+        <v>100</v>
+      </c>
+      <c r="G38" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="H38" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I38" s="24">
+        <v>0</v>
+      </c>
+      <c r="J38" s="22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="10">
+        <f>SUM(F2:F38)</f>
+        <v>932.64</v>
+      </c>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="11">
+        <f>SUM(I2:I38)</f>
+        <v>1010.25</v>
+      </c>
+      <c r="J39" s="9"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="I40" s="4">
+        <f>CONVERT(I39,"g","lbm")</f>
+        <v>2.2272200037227257</v>
+      </c>
+      <c r="J40" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="D33" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="F33" s="16">
-        <v>60</v>
-      </c>
-      <c r="G33" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="H33" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="I33" s="17">
-        <v>0</v>
-      </c>
-      <c r="J33" s="15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" s="22" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D34" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="E34" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="F34" s="23">
-        <v>100</v>
-      </c>
-      <c r="G34" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="H34" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="I34" s="24">
-        <v>0</v>
-      </c>
-      <c r="J34" s="22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="10">
-        <f>SUM(F2:F34)</f>
-        <v>902.1</v>
-      </c>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="11">
-        <f>SUM(I2:I34)</f>
-        <v>924.25</v>
-      </c>
-      <c r="J35" s="9"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="5" t="s">
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" s="21">
+        <f>SUM(F2:F21)</f>
+        <v>506.07</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="I36" s="4">
-        <f>CONVERT(I35,"g","lbm")</f>
-        <v>2.0376224582437308</v>
-      </c>
-      <c r="J36" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="B37" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B38" s="21">
-        <f>SUM(F2:F16)</f>
-        <v>467.54999999999995</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B39" s="21">
-        <f>SUM(F33:F34)</f>
+      <c r="B43" s="21">
+        <f>SUM(F37:F38)</f>
         <v>160</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="B40" s="25">
-        <f>SUM(F17:F27)</f>
+    <row r="44" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" s="25">
+        <f>SUM(F22:F32)</f>
         <v>238.95999999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B41" s="19">
-        <f>SUM(B38:B40)</f>
-        <v>866.51</v>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45" s="19">
+        <f>SUM(B42:B44)</f>
+        <v>905.03</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:G34">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="On Hand">
+  <conditionalFormatting sqref="G13:G16 G18:G38 G2:G11">
+    <cfRule type="containsText" dxfId="17" priority="7" operator="containsText" text="On Hand">
       <formula>NOT(ISERROR(SEARCH("On Hand",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Shipping">
+    <cfRule type="containsText" dxfId="16" priority="8" operator="containsText" text="Shipping">
       <formula>NOT(ISERROR(SEARCH("Shipping",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Hold">
+    <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="Hold">
       <formula>NOT(ISERROR(SEARCH("Hold",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G17">
+    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="On Hand">
+      <formula>NOT(ISERROR(SEARCH("On Hand",G17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="Shipping">
+      <formula>NOT(ISERROR(SEARCH("Shipping",G17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="Hold">
+      <formula>NOT(ISERROR(SEARCH("Hold",G17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="On Hand">
+      <formula>NOT(ISERROR(SEARCH("On Hand",G12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="Shipping">
+      <formula>NOT(ISERROR(SEARCH("Shipping",G12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Hold">
+      <formula>NOT(ISERROR(SEARCH("Hold",G12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="J23" r:id="rId1" xr:uid="{48D2BFA4-C137-8C46-BB60-E1F8938E8CA2}"/>
-    <hyperlink ref="J7" r:id="rId2" xr:uid="{CB2E9E6A-B2D9-BD4F-8E4A-C232CC8C6188}"/>
-    <hyperlink ref="J16" r:id="rId3" xr:uid="{05191A8A-B647-2B4F-BD0E-E5BA7E07A24D}"/>
-    <hyperlink ref="J31" r:id="rId4" xr:uid="{4B8FFD00-98BB-5948-A589-B4A08F4DD0AB}"/>
-    <hyperlink ref="J10" r:id="rId5" xr:uid="{9B176922-D2F1-5643-886E-36B3D6CE9370}"/>
+    <hyperlink ref="J28" r:id="rId1" xr:uid="{48D2BFA4-C137-8C46-BB60-E1F8938E8CA2}"/>
+    <hyperlink ref="J21" r:id="rId2" xr:uid="{05191A8A-B647-2B4F-BD0E-E5BA7E07A24D}"/>
+    <hyperlink ref="J35" r:id="rId3" xr:uid="{4B8FFD00-98BB-5948-A589-B4A08F4DD0AB}"/>
+    <hyperlink ref="J11" r:id="rId4" xr:uid="{9B176922-D2F1-5643-886E-36B3D6CE9370}"/>
+    <hyperlink ref="J19" r:id="rId5" xr:uid="{171B49AA-7673-FA40-BF5A-96C78B800495}"/>
+    <hyperlink ref="J14" r:id="rId6" xr:uid="{E26FF23A-AD12-3D47-B482-FDD0F8ECCC12}"/>
+    <hyperlink ref="J8" r:id="rId7" xr:uid="{1AF97322-C8B2-9642-9FAD-1F84CE809E30}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2223,16 +2604,207 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5DA0194-3BD8-0445-A0DA-BFF428184CF3}">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA48F912-73D5-C948-8F03-182370250086}">
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView zoomScale="113" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="53.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" customWidth="1"/>
+    <col min="10" max="10" width="135.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="27" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="32">
+        <v>33.19</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="17">
+        <v>10</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" s="32">
+        <v>10</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="17">
+        <v>10</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="16">
+        <v>4.07</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="17">
+        <v>10</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="G2">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="On Hand">
+      <formula>NOT(ISERROR(SEARCH("On Hand",G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Shipping">
+      <formula>NOT(ISERROR(SEARCH("Shipping",G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Hold">
+      <formula>NOT(ISERROR(SEARCH("Hold",G2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="On Hand">
+      <formula>NOT(ISERROR(SEARCH("On Hand",G3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Shipping">
+      <formula>NOT(ISERROR(SEARCH("Shipping",G3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Hold">
+      <formula>NOT(ISERROR(SEARCH("Hold",G3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="On Hand">
+      <formula>NOT(ISERROR(SEARCH("On Hand",G4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Shipping">
+      <formula>NOT(ISERROR(SEARCH("Shipping",G4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Hold">
+      <formula>NOT(ISERROR(SEARCH("Hold",G4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="J4" r:id="rId1" xr:uid="{A0DEF24D-33C1-4C4E-B965-14199C131A54}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5DA0194-3BD8-0445-A0DA-BFF428184CF3}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" customWidth="1"/>
     <col min="3" max="3" width="25.33203125" customWidth="1"/>
     <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
@@ -2245,30 +2817,30 @@
         <v>2</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>111</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D2" s="7">
         <v>44125</v>
@@ -2282,13 +2854,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="33" t="s">
         <v>119</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>120</v>
       </c>
       <c r="D3" s="7">
         <v>44125</v>
@@ -2302,13 +2874,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D4" s="7">
         <v>44126</v>
@@ -2322,10 +2894,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" t="s">
         <v>122</v>
-      </c>
-      <c r="B5" t="s">
-        <v>123</v>
       </c>
       <c r="D5" s="7">
         <v>44126</v>
@@ -2339,13 +2911,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" s="33" t="s">
         <v>123</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>124</v>
       </c>
       <c r="D6" s="7">
         <v>44126</v>
@@ -2359,13 +2931,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="33" t="s">
         <v>128</v>
-      </c>
-      <c r="B7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>129</v>
       </c>
       <c r="D7" s="7">
         <v>44130</v>
@@ -2379,7 +2951,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D8" s="7">
         <v>44145</v>
@@ -2393,13 +2965,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D9" s="7">
         <v>44145</v>
@@ -2413,13 +2985,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D10" s="7">
         <v>44145</v>
@@ -2433,10 +3005,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D11" s="7">
         <v>44145</v>
@@ -2446,6 +3018,40 @@
       </c>
       <c r="F11" s="7">
         <v>44148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>158</v>
+      </c>
+      <c r="B12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="D12" s="7">
+        <v>44165</v>
+      </c>
+      <c r="E12" s="7">
+        <v>44169</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="D13" s="7">
+        <v>44165</v>
+      </c>
+      <c r="E13" s="7">
+        <v>44168</v>
       </c>
     </row>
   </sheetData>
@@ -2457,6 +3063,8 @@
     <hyperlink ref="C7" r:id="rId5" xr:uid="{7140A5F8-B8BC-EF4D-AF29-E9452A95E33E}"/>
     <hyperlink ref="C9" r:id="rId6" xr:uid="{CD790371-B5F1-8343-B6A6-25001FA24401}"/>
     <hyperlink ref="C10" r:id="rId7" xr:uid="{8F8D2B3E-D3AF-0042-91EA-47811C63C6CB}"/>
+    <hyperlink ref="C12" r:id="rId8" xr:uid="{B1ACF10A-9B93-B649-AE83-14CB1DE57DF4}"/>
+    <hyperlink ref="C13" r:id="rId9" xr:uid="{E42F7CDF-91E4-B646-9D54-33B03A99D90D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Added Flight 2 information.
</commit_message>
<xml_diff>
--- a/documentation/bom.xlsx
+++ b/documentation/bom.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtc0030/Documents/Projects/HAB/ros-hab-dcs/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tigermailauburn-my.sharepoint.com/personal/mtc0030_auburn_edu/Documents/Documents/09_HAB/ros-hab-dcs/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367897F9-D06D-D348-92B5-AFD92E65E42E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{367897F9-D06D-D348-92B5-AFD92E65E42E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BD08888F-D940-B548-8457-F04A6B2689B8}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19480" activeTab="2" xr2:uid="{9E5CD0A4-BAAD-3342-BAB6-1E57A22FEC73}"/>
+    <workbookView xWindow="-35340" yWindow="920" windowWidth="33600" windowHeight="19480" activeTab="2" xr2:uid="{9E5CD0A4-BAAD-3342-BAB6-1E57A22FEC73}"/>
   </bookViews>
   <sheets>
     <sheet name="Flight 1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="225">
   <si>
     <t>Component</t>
   </si>
@@ -596,12 +596,6 @@
     <t>Battery Holder 6X 1.5V AA Battery Storage</t>
   </si>
   <si>
-    <t>Hold</t>
-  </si>
-  <si>
-    <t>Storage bins</t>
-  </si>
-  <si>
     <t>Shipping</t>
   </si>
   <si>
@@ -668,18 +662,9 @@
     <t>https://amz.run/4KEO</t>
   </si>
   <si>
-    <t>https://www.lowesforpros.com/pd/Hefty-8-5-Gallon-34-Quart-Clear-Base-with-White-Lid-Tote-with-Latching-Lid/1000505535</t>
-  </si>
-  <si>
     <t>Lowes</t>
   </si>
   <si>
-    <t xml:space="preserve">Hefty 8.5-Gallon (34-Quart) Clear Base with White Lid Tote </t>
-  </si>
-  <si>
-    <t>At Lowes</t>
-  </si>
-  <si>
     <t>Pickup</t>
   </si>
   <si>
@@ -692,13 +677,31 @@
     <t>Amazon (SN01 Main)</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>"1Z71EY050396674100"</t>
   </si>
   <si>
     <t>"979445244742"</t>
+  </si>
+  <si>
+    <t>"420368499305520207600181455935"</t>
+  </si>
+  <si>
+    <t>Ublox MAX-M8Q</t>
+  </si>
+  <si>
+    <t>AirSpy.US</t>
+  </si>
+  <si>
+    <t>https://v3.airspy.us/product/upu-ublox-m8q3a-sma/</t>
+  </si>
+  <si>
+    <t>unused</t>
+  </si>
+  <si>
+    <t>AirSpy</t>
+  </si>
+  <si>
+    <t>"9405511202537835173094"</t>
   </si>
 </sst>
 </file>
@@ -831,7 +834,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -872,13 +875,24 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="62">
+  <dxfs count="63">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -2471,7 +2485,7 @@
         <v>20</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D23" s="29" t="s">
         <v>10</v>
@@ -2489,7 +2503,7 @@
         <v>5</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -3125,250 +3139,250 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F10:F12 F2:F8 F15:F38">
-    <cfRule type="containsText" dxfId="61" priority="70" operator="containsText" text="On Hand">
+    <cfRule type="containsText" dxfId="62" priority="70" operator="containsText" text="On Hand">
       <formula>NOT(ISERROR(SEARCH("On Hand",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="71" operator="containsText" text="Shipping">
+    <cfRule type="containsText" dxfId="61" priority="71" operator="containsText" text="Shipping">
       <formula>NOT(ISERROR(SEARCH("Shipping",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="72" operator="containsText" text="Hold">
+    <cfRule type="containsText" dxfId="60" priority="72" operator="containsText" text="Hold">
       <formula>NOT(ISERROR(SEARCH("Hold",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30">
-    <cfRule type="containsText" dxfId="58" priority="67" operator="containsText" text="On Hand">
+    <cfRule type="containsText" dxfId="59" priority="67" operator="containsText" text="On Hand">
       <formula>NOT(ISERROR(SEARCH("On Hand",F30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="68" operator="containsText" text="Shipping">
+    <cfRule type="containsText" dxfId="58" priority="68" operator="containsText" text="Shipping">
       <formula>NOT(ISERROR(SEARCH("Shipping",F30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="69" operator="containsText" text="Hold">
+    <cfRule type="containsText" dxfId="57" priority="69" operator="containsText" text="Hold">
       <formula>NOT(ISERROR(SEARCH("Hold",F30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F39">
-    <cfRule type="containsText" dxfId="55" priority="21" operator="containsText" text="On Hand">
+    <cfRule type="containsText" dxfId="56" priority="21" operator="containsText" text="On Hand">
       <formula>NOT(ISERROR(SEARCH("On Hand",F39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="22" operator="containsText" text="Shipping">
+    <cfRule type="containsText" dxfId="55" priority="22" operator="containsText" text="Shipping">
       <formula>NOT(ISERROR(SEARCH("Shipping",F39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="23" operator="containsText" text="Hold">
+    <cfRule type="containsText" dxfId="54" priority="23" operator="containsText" text="Hold">
       <formula>NOT(ISERROR(SEARCH("Hold",F39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22:F28">
-    <cfRule type="containsText" dxfId="52" priority="57" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="53" priority="57" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="containsText" dxfId="51" priority="56" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="52" priority="56" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23:F28">
-    <cfRule type="containsText" dxfId="50" priority="24" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="51" priority="24" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="containsText" dxfId="49" priority="55" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="50" priority="55" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="containsText" dxfId="48" priority="54" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="49" priority="54" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="containsText" dxfId="47" priority="53" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="48" priority="53" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="containsText" dxfId="46" priority="52" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="47" priority="52" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="containsText" dxfId="45" priority="51" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="46" priority="51" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F36">
-    <cfRule type="containsText" dxfId="44" priority="50" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="45" priority="50" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="containsText" dxfId="43" priority="47" operator="containsText" text="On Hand">
+    <cfRule type="containsText" dxfId="44" priority="47" operator="containsText" text="On Hand">
       <formula>NOT(ISERROR(SEARCH("On Hand",F9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="48" operator="containsText" text="Shipping">
+    <cfRule type="containsText" dxfId="43" priority="48" operator="containsText" text="Shipping">
       <formula>NOT(ISERROR(SEARCH("Shipping",F9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="49" operator="containsText" text="Hold">
+    <cfRule type="containsText" dxfId="42" priority="49" operator="containsText" text="Hold">
       <formula>NOT(ISERROR(SEARCH("Hold",F9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="containsText" dxfId="40" priority="46" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="41" priority="46" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="containsText" dxfId="39" priority="45" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="40" priority="45" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="containsText" dxfId="38" priority="44" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="39" priority="44" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="containsText" dxfId="37" priority="43" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="38" priority="43" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="containsText" dxfId="36" priority="40" operator="containsText" text="On Hand">
+    <cfRule type="containsText" dxfId="37" priority="40" operator="containsText" text="On Hand">
       <formula>NOT(ISERROR(SEARCH("On Hand",F13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="41" operator="containsText" text="Shipping">
+    <cfRule type="containsText" dxfId="36" priority="41" operator="containsText" text="Shipping">
       <formula>NOT(ISERROR(SEARCH("Shipping",F13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="42" operator="containsText" text="Hold">
+    <cfRule type="containsText" dxfId="35" priority="42" operator="containsText" text="Hold">
       <formula>NOT(ISERROR(SEARCH("Hold",F13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="containsText" dxfId="33" priority="39" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="34" priority="39" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="containsText" dxfId="32" priority="36" operator="containsText" text="On Hand">
+    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="On Hand">
       <formula>NOT(ISERROR(SEARCH("On Hand",F14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="37" operator="containsText" text="Shipping">
+    <cfRule type="containsText" dxfId="32" priority="37" operator="containsText" text="Shipping">
       <formula>NOT(ISERROR(SEARCH("Shipping",F14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="38" operator="containsText" text="Hold">
+    <cfRule type="containsText" dxfId="31" priority="38" operator="containsText" text="Hold">
       <formula>NOT(ISERROR(SEARCH("Hold",F14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="containsText" dxfId="29" priority="35" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="30" priority="35" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="containsText" dxfId="28" priority="34" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="29" priority="34" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="containsText" dxfId="27" priority="33" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="28" priority="33" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17">
-    <cfRule type="containsText" dxfId="26" priority="32" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="27" priority="32" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="containsText" dxfId="25" priority="31" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="26" priority="31" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19">
-    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="25" priority="30" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20">
-    <cfRule type="containsText" dxfId="23" priority="29" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="24" priority="29" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21">
-    <cfRule type="containsText" dxfId="22" priority="28" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="23" priority="28" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24:F28">
-    <cfRule type="containsText" dxfId="21" priority="26" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F26">
-    <cfRule type="containsText" dxfId="20" priority="25" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="21" priority="25" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42">
-    <cfRule type="containsText" dxfId="19" priority="18" operator="containsText" text="On Hand">
+    <cfRule type="containsText" dxfId="20" priority="18" operator="containsText" text="On Hand">
       <formula>NOT(ISERROR(SEARCH("On Hand",F42)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="Shipping">
+    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="Shipping">
       <formula>NOT(ISERROR(SEARCH("Shipping",F42)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="20" operator="containsText" text="Hold">
+    <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="Hold">
       <formula>NOT(ISERROR(SEARCH("Hold",F42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F40">
-    <cfRule type="containsText" dxfId="16" priority="15" operator="containsText" text="On Hand">
+    <cfRule type="containsText" dxfId="17" priority="15" operator="containsText" text="On Hand">
       <formula>NOT(ISERROR(SEARCH("On Hand",F40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="Shipping">
+    <cfRule type="containsText" dxfId="16" priority="16" operator="containsText" text="Shipping">
       <formula>NOT(ISERROR(SEARCH("Shipping",F40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="17" operator="containsText" text="Hold">
+    <cfRule type="containsText" dxfId="15" priority="17" operator="containsText" text="Hold">
       <formula>NOT(ISERROR(SEARCH("Hold",F40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F41">
-    <cfRule type="containsText" dxfId="13" priority="12" operator="containsText" text="On Hand">
+    <cfRule type="containsText" dxfId="14" priority="12" operator="containsText" text="On Hand">
       <formula>NOT(ISERROR(SEARCH("On Hand",F41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="Shipping">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="Shipping">
       <formula>NOT(ISERROR(SEARCH("Shipping",F41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="14" operator="containsText" text="Hold">
+    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="Hold">
       <formula>NOT(ISERROR(SEARCH("Hold",F41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F27">
-    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="On Hand">
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="On Hand">
       <formula>NOT(ISERROR(SEARCH("On Hand",F27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="Shipping">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Shipping">
       <formula>NOT(ISERROR(SEARCH("Shipping",F27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="Hold">
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Hold">
       <formula>NOT(ISERROR(SEARCH("Hold",F27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F27">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25:F28">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="consumed">
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="consumed">
       <formula>NOT(ISERROR(SEARCH("consumed",F25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F25)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3393,7 +3407,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView zoomScale="113" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3480,7 +3494,7 @@
         <v>32.99</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>191</v>
+        <v>103</v>
       </c>
       <c r="G3" s="16" t="s">
         <v>19</v>
@@ -3509,7 +3523,7 @@
         <v>27.99</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>191</v>
+        <v>103</v>
       </c>
       <c r="G4" s="16" t="s">
         <v>19</v>
@@ -3538,7 +3552,7 @@
         <v>10.06</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>191</v>
+        <v>103</v>
       </c>
       <c r="G5" s="16" t="s">
         <v>19</v>
@@ -3558,7 +3572,7 @@
         <v>20</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>91</v>
@@ -3567,7 +3581,7 @@
         <v>55</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>191</v>
+        <v>103</v>
       </c>
       <c r="G6" s="16" t="s">
         <v>19</v>
@@ -3576,7 +3590,7 @@
         <v>20</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -3596,7 +3610,7 @@
         <v>5.97</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>191</v>
+        <v>103</v>
       </c>
       <c r="G7" s="16" t="s">
         <v>19</v>
@@ -3625,7 +3639,7 @@
         <v>14.3</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>191</v>
+        <v>103</v>
       </c>
       <c r="G8" s="16" t="s">
         <v>19</v>
@@ -3639,13 +3653,13 @@
     </row>
     <row r="9" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>94</v>
@@ -3654,7 +3668,7 @@
         <v>9.9499999999999993</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>191</v>
+        <v>103</v>
       </c>
       <c r="G9" s="16" t="s">
         <v>19</v>
@@ -3663,7 +3677,7 @@
         <v>10</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -3683,7 +3697,7 @@
         <v>19.95</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>191</v>
+        <v>103</v>
       </c>
       <c r="G10" s="16" t="s">
         <v>19</v>
@@ -3712,7 +3726,7 @@
         <v>14.95</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>191</v>
+        <v>103</v>
       </c>
       <c r="G11" s="16" t="s">
         <v>19</v>
@@ -3741,7 +3755,7 @@
         <v>9.9499999999999993</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>191</v>
+        <v>103</v>
       </c>
       <c r="G12" s="16" t="s">
         <v>19</v>
@@ -3755,158 +3769,158 @@
     </row>
     <row r="13" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>187</v>
+        <v>158</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="E13" s="30">
-        <v>39.99</v>
+        <v>14.99</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>191</v>
+        <v>103</v>
       </c>
       <c r="G13" s="16" t="s">
         <v>19</v>
       </c>
       <c r="H13" s="17">
+        <v>20</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="18" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="29" t="s">
-        <v>159</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>158</v>
-      </c>
-      <c r="D14" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="30">
-        <v>14.99</v>
+      <c r="E14" s="16">
+        <v>99.99</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>191</v>
+        <v>103</v>
       </c>
       <c r="G14" s="16" t="s">
         <v>19</v>
       </c>
       <c r="H14" s="17">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>160</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
-        <v>33</v>
+      <c r="A15" s="29" t="s">
+        <v>121</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="15" t="s">
+      <c r="C15" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="D15" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="16">
-        <v>99.99</v>
+      <c r="E15" s="30">
+        <v>10.59</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>191</v>
+        <v>103</v>
       </c>
       <c r="G15" s="16" t="s">
         <v>19</v>
       </c>
       <c r="H15" s="17">
-        <v>87</v>
+        <v>15</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>34</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="29" t="s">
-        <v>121</v>
+      <c r="A16" s="15" t="s">
+        <v>44</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="29" t="s">
-        <v>208</v>
-      </c>
-      <c r="D16" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="30">
-        <v>10.59</v>
+      <c r="C16" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E16" s="16">
+        <v>2.5</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>191</v>
+        <v>103</v>
       </c>
       <c r="G16" s="16" t="s">
         <v>19</v>
       </c>
       <c r="H16" s="17">
-        <v>15</v>
-      </c>
-      <c r="I16" s="18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E17" s="16">
-        <v>2.5</v>
+        <v>20</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="E17" s="27">
+        <v>40.950000000000003</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G17" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="H17" s="17">
-        <v>20</v>
-      </c>
-      <c r="I17" s="15" t="s">
-        <v>210</v>
+      <c r="H17" s="28">
+        <v>10</v>
+      </c>
+      <c r="I17" s="34" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="26" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B18" s="26" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D18" s="26" t="s">
         <v>41</v>
@@ -3915,7 +3929,7 @@
         <v>199.99</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G18" s="16" t="s">
         <v>19</v>
@@ -3924,7 +3938,7 @@
         <v>30</v>
       </c>
       <c r="I18" s="26" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.2">
@@ -3944,7 +3958,7 @@
         <v>35</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G19" s="16" t="s">
         <v>30</v>
@@ -3964,7 +3978,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>10</v>
@@ -3973,7 +3987,7 @@
         <v>12.78</v>
       </c>
       <c r="F20" s="27" t="s">
-        <v>191</v>
+        <v>103</v>
       </c>
       <c r="G20" s="16" t="s">
         <v>30</v>
@@ -3983,7 +3997,7 @@
         <v>138</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -4003,7 +4017,7 @@
         <v>59.85</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G21" s="16" t="s">
         <v>30</v>
@@ -4046,13 +4060,13 @@
     </row>
     <row r="23" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>57</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>10</v>
@@ -4061,7 +4075,7 @@
         <v>10.59</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>191</v>
+        <v>103</v>
       </c>
       <c r="G23" s="16" t="s">
         <v>23</v>
@@ -4070,27 +4084,27 @@
         <v>0</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="B24" s="15" t="s">
         <v>57</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>214</v>
+        <v>10</v>
       </c>
       <c r="E24" s="16">
-        <v>17.96</v>
+        <v>24.86</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>216</v>
+        <v>103</v>
       </c>
       <c r="G24" s="16" t="s">
         <v>23</v>
@@ -4099,36 +4113,36 @@
         <v>0</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="15" t="s">
-        <v>199</v>
+      <c r="A25" s="29" t="s">
+        <v>171</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="D25" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" s="30">
+        <v>39.99</v>
+      </c>
+      <c r="F25" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H25" s="17">
         <v>10</v>
       </c>
-      <c r="E25" s="16">
-        <v>24.86</v>
-      </c>
-      <c r="F25" s="27" t="s">
-        <v>191</v>
-      </c>
-      <c r="G25" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H25" s="17">
-        <v>0</v>
-      </c>
       <c r="I25" s="18" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -4147,8 +4161,8 @@
       <c r="E26" s="16">
         <v>15</v>
       </c>
-      <c r="F26" s="16" t="s">
-        <v>189</v>
+      <c r="F26" s="27" t="s">
+        <v>103</v>
       </c>
       <c r="G26" s="16" t="s">
         <v>23</v>
@@ -4169,7 +4183,7 @@
       <c r="D27" s="9"/>
       <c r="E27" s="10">
         <f>SUM(E2:E26)</f>
-        <v>825.2</v>
+        <v>848.18999999999994</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
@@ -4209,7 +4223,7 @@
       </c>
       <c r="B30" s="21">
         <f>SUM(E2:E18)</f>
-        <v>569.16</v>
+        <v>570.11999999999989</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -4227,7 +4241,7 @@
       </c>
       <c r="B32" s="23">
         <f>SUM(E23:E26)</f>
-        <v>68.41</v>
+        <v>90.44</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -4236,30 +4250,36 @@
       </c>
       <c r="B33" s="19">
         <f>SUM(B30:B32)</f>
-        <v>825.19999999999993</v>
+        <v>848.18999999999983</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F26">
-    <cfRule type="containsText" dxfId="3" priority="56" operator="containsText" text="On Hand">
+    <cfRule type="containsText" dxfId="4" priority="57" operator="containsText" text="On Hand">
       <formula>NOT(ISERROR(SEARCH("On Hand",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="57" operator="containsText" text="Shipping">
+    <cfRule type="containsText" dxfId="3" priority="58" operator="containsText" text="Shipping">
       <formula>NOT(ISERROR(SEARCH("Shipping",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="58" operator="containsText" text="Hold">
+    <cfRule type="containsText" dxfId="2" priority="59" operator="containsText" text="Hold">
       <formula>NOT(ISERROR(SEARCH("Hold",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F25">
-    <cfRule type="containsText" dxfId="0" priority="51" operator="containsText" text="on payload">
+    <cfRule type="containsText" dxfId="1" priority="52" operator="containsText" text="on payload">
       <formula>NOT(ISERROR(SEARCH("on payload",F2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F26">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="on payload">
+      <formula>NOT(ISERROR(SEARCH("on payload",F26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="I15" r:id="rId1" xr:uid="{2F93E9C5-DDF9-5F4D-AC8B-0138CD920BDD}"/>
-    <hyperlink ref="I14" r:id="rId2" xr:uid="{79B0F088-7F49-DC45-9273-1E98B495DCAA}"/>
+    <hyperlink ref="I14" r:id="rId1" xr:uid="{2F93E9C5-DDF9-5F4D-AC8B-0138CD920BDD}"/>
+    <hyperlink ref="I13" r:id="rId2" xr:uid="{79B0F088-7F49-DC45-9273-1E98B495DCAA}"/>
     <hyperlink ref="I9" r:id="rId3" xr:uid="{D98D00E4-F901-C34C-901A-5594B9C3661A}"/>
+    <hyperlink ref="I17" r:id="rId4" xr:uid="{DFA6AA16-D506-5143-A0ED-671601E48814}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4268,10 +4288,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5DA0194-3BD8-0445-A0DA-BFF428184CF3}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4346,7 +4366,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B4" t="s">
         <v>115</v>
@@ -4535,7 +4555,7 @@
     <row r="14" spans="1:6" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D15" s="7">
         <v>44246</v>
@@ -4543,19 +4563,23 @@
       <c r="E15" s="7">
         <v>44249</v>
       </c>
-      <c r="F15" s="7"/>
+      <c r="F15" s="7">
+        <v>44251</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D16" s="7">
         <v>44246</v>
       </c>
       <c r="E16" s="7">
-        <v>44253</v>
-      </c>
-      <c r="F16" s="7"/>
+        <v>44252</v>
+      </c>
+      <c r="F16" s="7">
+        <v>44252</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -4565,7 +4589,7 @@
         <v>115</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="D17" s="7">
         <v>44246</v>
@@ -4573,7 +4597,9 @@
       <c r="E17" s="7">
         <v>44252</v>
       </c>
-      <c r="F17" s="7"/>
+      <c r="F17" s="7">
+        <v>44252</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -4583,7 +4609,7 @@
         <v>112</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="D18" s="7">
         <v>44246</v>
@@ -4591,14 +4617,16 @@
       <c r="E18" s="7">
         <v>44251</v>
       </c>
-      <c r="F18" s="7"/>
+      <c r="F18" s="7">
+        <v>44252</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B19" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D19" s="7">
         <v>44246</v>
@@ -4617,11 +4645,28 @@
       <c r="B20" t="s">
         <v>111</v>
       </c>
+      <c r="C20" s="31" t="s">
+        <v>218</v>
+      </c>
       <c r="D20" s="7">
         <v>44242</v>
       </c>
-      <c r="E20" s="7" t="s">
-        <v>221</v>
+      <c r="E20" s="7">
+        <v>44256</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>223</v>
+      </c>
+      <c r="B21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="D21" s="7">
+        <v>44256</v>
       </c>
     </row>
   </sheetData>
@@ -4637,6 +4682,8 @@
     <hyperlink ref="C13" r:id="rId9" xr:uid="{E42F7CDF-91E4-B646-9D54-33B03A99D90D}"/>
     <hyperlink ref="C17" r:id="rId10" xr:uid="{8C2FEC4C-3BA2-5440-906A-4E5201E0D31B}"/>
     <hyperlink ref="C18" r:id="rId11" xr:uid="{88B72672-F97F-F34B-9A42-2CECA5A055E9}"/>
+    <hyperlink ref="C20" r:id="rId12" xr:uid="{734E0666-91BE-E146-B4AF-3A6E22A0239D}"/>
+    <hyperlink ref="C21" r:id="rId13" xr:uid="{F469FC70-5A60-5041-A0F4-6699B3949F24}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>